<commit_message>
changing wrf run script for MPIEXEX Capture
</commit_message>
<xml_diff>
--- a/namelist_files_and_local_scripts/time_series_station_files_3_dom_all.xlsx
+++ b/namelist_files_and_local_scripts/time_series_station_files_3_dom_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/SD_Mines_WRF_REALTIME/namelist_files_and_local_scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B164D802-C55A-C24B-802D-BC5AA1AEE34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFBD062-6C33-7D4E-8A5A-A993133F515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,14 +234,14 @@
     <t>Philip Arpt, SD</t>
   </si>
   <si>
-    <t>Distane from UNR</t>
+    <t>Distane from SDMines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +260,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -316,9 +323,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +632,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -632,7 +640,7 @@
     <col min="1" max="2" width="30.1640625" customWidth="1"/>
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="6" width="30.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -658,7 +666,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>26</v>
       </c>
@@ -677,11 +685,11 @@
       <c r="F2">
         <v>-103.211</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="4">
+        <v>0.44024747661156699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>21</v>
       </c>
@@ -700,11 +708,11 @@
       <c r="F3">
         <v>-103.1</v>
       </c>
-      <c r="G3">
-        <v>1.5957090000001551E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="4">
+        <v>10.688774683141601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -723,11 +731,11 @@
       <c r="F4">
         <v>-103.054</v>
       </c>
-      <c r="G4">
-        <v>2.5531089999998792E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="4">
+        <v>12.624086669234799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>25</v>
       </c>
@@ -746,11 +754,11 @@
       <c r="F5">
         <v>-102.833</v>
       </c>
-      <c r="G5">
-        <v>0.14652009000000071</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="4">
+        <v>30.4844243744819</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7</v>
       </c>
@@ -769,11 +777,11 @@
       <c r="F6">
         <v>-103.611</v>
       </c>
-      <c r="G6">
-        <v>0.27539609000000492</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="4">
+        <v>49.927563605199097</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>23</v>
       </c>
@@ -792,11 +800,11 @@
       <c r="F7">
         <v>-103.783</v>
       </c>
-      <c r="G7">
-        <v>0.4955300900000027</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="4">
+        <v>64.629982737682198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>10</v>
       </c>
@@ -815,149 +823,149 @@
       <c r="F8">
         <v>-103.86199999999999</v>
       </c>
-      <c r="G8">
-        <v>0.86111869000000074</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" s="4">
+        <v>89.994937722499401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>44.6629</v>
+      </c>
+      <c r="F9">
+        <v>-104.568</v>
+      </c>
+      <c r="G9" s="4">
+        <v>126.519155018898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>44.051000000000002</v>
+      </c>
+      <c r="F10">
+        <v>-101.601</v>
+      </c>
+      <c r="G10" s="4">
+        <v>128.259606930252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11">
+        <v>43.021000000000001</v>
+      </c>
+      <c r="F11">
+        <v>-102.518</v>
+      </c>
+      <c r="G11" s="4">
+        <v>129.56952994696701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9">
+      <c r="E12">
         <v>42.837000000000003</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>-103.098</v>
       </c>
-      <c r="G9">
-        <v>1.5397234899999857</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="G12" s="4">
+        <v>137.845928181538</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>44.267000000000003</v>
+      </c>
+      <c r="F13">
+        <v>-104.95</v>
+      </c>
+      <c r="G13" s="4">
+        <v>140.74316527471001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10">
-        <v>43.021000000000001</v>
-      </c>
-      <c r="F10">
-        <v>-102.518</v>
-      </c>
-      <c r="G10">
-        <v>1.5863218899999902</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11">
-        <v>44.6629</v>
-      </c>
-      <c r="F11">
-        <v>-104.568</v>
-      </c>
-      <c r="G11">
-        <v>2.1897850400000016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E12">
+      <c r="E14">
         <v>45.031999999999996</v>
       </c>
-      <c r="F12">
+      <c r="F14">
         <v>-102.01900000000001</v>
       </c>
-      <c r="G12">
-        <v>2.3411204899999816</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13">
-        <v>45.603999999999999</v>
-      </c>
-      <c r="F13">
-        <v>-103.54600000000001</v>
-      </c>
-      <c r="G13">
-        <v>2.4571046900000106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14">
-        <v>44.051000000000002</v>
-      </c>
-      <c r="F14">
-        <v>-101.601</v>
-      </c>
-      <c r="G14">
-        <v>2.592570889999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G14" s="4">
+        <v>142.08000880628899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -976,287 +984,287 @@
       <c r="F15">
         <v>-102.175</v>
       </c>
-      <c r="G15">
-        <v>2.6778248900000032</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G15" s="4">
+        <v>163.745344265017</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16">
-        <v>44.267000000000003</v>
+        <v>45.603999999999999</v>
       </c>
       <c r="F16">
-        <v>-104.95</v>
-      </c>
-      <c r="G16">
-        <v>3.0618734900000173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-103.54600000000001</v>
+      </c>
+      <c r="G16" s="4">
+        <v>172.20643453350701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>44.338999999999999</v>
+      </c>
+      <c r="F17">
+        <v>-105.542</v>
+      </c>
+      <c r="G17" s="4">
+        <v>188.51267235667501</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>46.017000000000003</v>
       </c>
-      <c r="F17">
+      <c r="F18">
         <v>-102.65</v>
       </c>
-      <c r="G17">
-        <v>4.0950234900000133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="G18" s="4">
+        <v>220.39859088188999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>45.933</v>
+      </c>
+      <c r="F19">
+        <v>-102.167</v>
+      </c>
+      <c r="G19" s="4">
+        <v>222.238034808328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20">
+        <v>45.918999999999997</v>
+      </c>
+      <c r="F20">
+        <v>-102.10599999999999</v>
+      </c>
+      <c r="G20" s="4">
+        <v>222.613286981622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21">
+        <v>42.795999999999999</v>
+      </c>
+      <c r="F21">
+        <v>-105.38</v>
+      </c>
+      <c r="G21" s="4">
+        <v>225.856416908353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>5</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18">
-        <v>42.05</v>
-      </c>
-      <c r="F18">
-        <v>-102.8</v>
-      </c>
-      <c r="G18">
-        <v>4.2602362900000026</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19">
-        <v>46.186999999999998</v>
-      </c>
-      <c r="F19">
-        <v>-103.428</v>
-      </c>
-      <c r="G19">
-        <v>4.5173534899999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20">
-        <v>45.933</v>
-      </c>
-      <c r="F20">
-        <v>-102.167</v>
-      </c>
-      <c r="G20">
-        <v>4.5506520900000016</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21">
-        <v>45.918999999999997</v>
-      </c>
-      <c r="F21">
-        <v>-102.10599999999999</v>
-      </c>
-      <c r="G21">
-        <v>4.6298486900000064</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <v>42.05</v>
+      </c>
+      <c r="F22">
+        <v>-102.8</v>
+      </c>
+      <c r="G22" s="4">
+        <v>227.482904000014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23">
+        <v>42.75</v>
+      </c>
+      <c r="F23">
+        <v>-105.383</v>
+      </c>
+      <c r="G23" s="4">
+        <v>229.34578734732301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24">
+        <v>42.433</v>
+      </c>
+      <c r="F24">
+        <v>-105.033</v>
+      </c>
+      <c r="G24" s="4">
+        <v>234.931316989593</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25">
+        <v>44.381</v>
+      </c>
+      <c r="F25">
+        <v>-100.286</v>
+      </c>
+      <c r="G25" s="4">
+        <v>235.13106135770599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <v>46.186999999999998</v>
+      </c>
+      <c r="F26">
+        <v>-103.428</v>
+      </c>
+      <c r="G26" s="4">
+        <v>235.57785564806699</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E22">
+      <c r="E27">
         <v>42.061</v>
       </c>
-      <c r="F22">
+      <c r="F27">
         <v>-104.158</v>
       </c>
-      <c r="G22">
-        <v>4.9437458899999962</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23">
-        <v>41.871000000000002</v>
-      </c>
-      <c r="F23">
-        <v>-103.593</v>
-      </c>
-      <c r="G23">
-        <v>4.9934068899999833</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>11</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24">
-        <v>44.338999999999999</v>
-      </c>
-      <c r="F24">
-        <v>-105.542</v>
-      </c>
-      <c r="G24">
-        <v>5.5044766900000148</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25">
-        <v>42.433</v>
-      </c>
-      <c r="F25">
-        <v>-105.033</v>
-      </c>
-      <c r="G25">
-        <v>6.0083000900000023</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26">
-        <v>42.795999999999999</v>
-      </c>
-      <c r="F26">
-        <v>-105.38</v>
-      </c>
-      <c r="G26">
-        <v>6.3345238899999821</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27">
-        <v>42.75</v>
-      </c>
-      <c r="F27">
-        <v>-105.383</v>
-      </c>
-      <c r="G27">
-        <v>6.4671192899999808</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" s="4">
+        <v>236.837322668903</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>17</v>
       </c>
@@ -1275,57 +1283,57 @@
       <c r="F28">
         <v>-100.617</v>
       </c>
-      <c r="G28">
-        <v>7.8098120899999612</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" s="4">
+        <v>238.58488715181201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29">
+        <v>41.871000000000002</v>
+      </c>
+      <c r="F29">
+        <v>-103.593</v>
+      </c>
+      <c r="G29" s="4">
+        <v>247.000180903119</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>25</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <v>42.878</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>-100.55</v>
       </c>
-      <c r="G29">
-        <v>8.5082290900000004</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30">
-        <v>44.381</v>
-      </c>
-      <c r="F30">
-        <v>-100.286</v>
-      </c>
-      <c r="G30">
-        <v>8.6506738899999842</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G30" s="4">
+        <v>252.207140948887</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1344,8 +1352,8 @@
       <c r="F31">
         <v>-98.834999999999994</v>
       </c>
-      <c r="G31">
-        <v>40.254212000000102</v>
+      <c r="G31" s="4">
+        <v>610.69674570044003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>